<commit_message>
motor_respuesta_v3.js v3.1 final — campañas + CTA + clínica
</commit_message>
<xml_diff>
--- a/Campañas.xlsx
+++ b/Campañas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juancarloscontreras/Zara-2.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{438D0BD7-A448-754E-AB9F-E1C569323746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2733ABF4-AB93-4F49-ABC5-8F0CA54864C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{E2898BD9-E948-B341-86E4-DBACD3E87737}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>id</t>
   </si>
@@ -53,59 +53,37 @@
     <t>saludo</t>
   </si>
   <si>
-    <t>descripcion</t>
-  </si>
-  <si>
-    <t>precio</t>
-  </si>
-  <si>
-    <t>sesiones</t>
-  </si>
-  <si>
-    <t>cta</t>
-  </si>
-  <si>
-    <t>Lipo Express Verano</t>
-  </si>
-  <si>
-    <t>whatsapp</t>
-  </si>
-  <si>
     <t>lipo express</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">¡Hola! 🌞 Vi que vienes por nuestra campaña </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lipo Express Verano</t>
-    </r>
-  </si>
-  <si>
-    <t>Reduce grasa y moldea cintura con HIFU 12D + Cavitación + RF</t>
-  </si>
-  <si>
-    <t>6 sesiones</t>
-  </si>
-  <si>
-    <t>Agenda tu evaluación gratuita aquí 👉 [link]</t>
-  </si>
-  <si>
-    <t>Face Elite Rejuvenece</t>
-  </si>
-  <si>
     <t>instagram</t>
   </si>
   <si>
-    <t>face elite</t>
+    <t>Push Up Glúteos</t>
+  </si>
+  <si>
+    <t>push up</t>
+  </si>
+  <si>
+    <t>¡Hola! Quiero más información sobre el Plan Push up</t>
+  </si>
+  <si>
+    <t>Mensaje llegada</t>
+  </si>
+  <si>
+    <t>¡Hola! 🌞 Vi que estas interesada en Push Up, 
+este es un  plan diseñado para levantar, dar volumen y mejorar la firmeza del glúteo. Combina Pro Sculpt (20.000 contracciones en 30 min), HIFU 12D para efecto tensor y Radiofrecuencia para compactar y definir.
+Los resultados comienzan a notarse desde las primeras semanas.
+Si quieres ajustar la cantidad de sesiones a tu caso, te dejo tu diagnóstico gratuito para evaluar volumen, firmeza y tu objetivo real:</t>
+  </si>
+  <si>
+    <t>Instagram</t>
+  </si>
+  <si>
+    <t>Quiero saber más de los tratamientos de lipo por un verano sin</t>
+  </si>
+  <si>
+    <t>un verano sin</t>
   </si>
   <si>
     <r>
@@ -120,45 +98,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Face Elite</t>
+      <t>nuestro tratamiento  Lipo Express, te cuento este es uno de nuestros planes favoritos porque entrega cambios visibles en poco tiempo ✨.
+Trabaja abdomen, cintura, flancos, brazos o piernas combinando tecnologías de alta potencia:
+• HIFU 12D para atacar grasa localizada profunda
+• Cavitación para romper adipocitos
+• Radiofrecuencia profunda para tensar y mejorar la firmeza
+• Pro Sculpt para esculpir y definir con 20.000 contracciones por sesión
+El resultado: una zona más definida, menos volumen y un contorno más firme.
+Cada cuerpo responde distinto, por eso la clave es partir con un diagnóstico gratuito donde revisamos tu punto de partida y te decimos cuántas sesiones realmente necesitas, sin venderte de más 💙.</t>
     </r>
   </si>
   <si>
-    <t>Tratamiento facial con Pink Glow, RF 12D y Toxina Botulínica Clínica</t>
-  </si>
-  <si>
-    <t>4 sesiones</t>
-  </si>
-  <si>
-    <t>Agenda tu diagnóstico con IA aquí 👉 [link]</t>
-  </si>
-  <si>
-    <t>Push Up Glúteos</t>
-  </si>
-  <si>
-    <t>push up</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">¡Hola! 🍑 Gracias por escribirnos por </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Push Up Glúteos</t>
-    </r>
-  </si>
-  <si>
-    <t>Levanta y tonifica con EMS Sculptor + RF profunda</t>
-  </si>
-  <si>
-    <t>Reserva tu evaluación gratis 👉 [link]</t>
+    <t>precio campaña</t>
   </si>
 </sst>
 </file>
@@ -168,7 +119,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -191,6 +142,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF1C1E21"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -219,10 +176,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -238,10 +199,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -561,25 +518,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68B99F10-75E4-F24D-AD2F-A01E2918D3DD}">
-  <dimension ref="B2:J5"/>
+  <dimension ref="B2:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="55.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="56.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="68.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -590,109 +545,62 @@
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:8" ht="136" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
       <c r="H3" s="1">
-        <v>432000</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" t="s">
-        <v>15</v>
+        <v>375990</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:8" ht="255" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
+        <v>5</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="H4" s="1">
-        <v>358400</v>
-      </c>
-      <c r="I4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="1">
-        <v>376000</v>
-      </c>
-      <c r="I5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" t="s">
-        <v>27</v>
+        <v>431990</v>
       </c>
     </row>
   </sheetData>

</xml_diff>